<commit_message>
Theme 3 is passed
</commit_message>
<xml_diff>
--- a/Lab3.1.xlsx
+++ b/Lab3.1.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Вручную" sheetId="1" r:id="rId1"/>
-    <sheet name="Отчет о результатах 1" sheetId="10" r:id="rId2"/>
-    <sheet name="Отчет об устойчивости 1" sheetId="11" r:id="rId3"/>
-    <sheet name="Отчет о пределах 1" sheetId="12" r:id="rId4"/>
+    <sheet name="Отчет о результатах 1" sheetId="13" r:id="rId2"/>
+    <sheet name="Отчет об устойчивости 1" sheetId="14" r:id="rId3"/>
+    <sheet name="Отчет о пределах 1" sheetId="15" r:id="rId4"/>
     <sheet name="Поиск решения" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -26,7 +26,7 @@
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="88">
   <si>
     <t>- заводские специалисты</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Microsoft Excel 16.0 Отчет о результатах</t>
   </si>
   <si>
-    <t>Лист: [Lab3.xlsx]Поиск решения</t>
-  </si>
-  <si>
     <t>Результат: Решение найдено. Все ограничения и условия оптимальности выполнены.</t>
   </si>
   <si>
@@ -226,15 +223,6 @@
     <t>$D$2&gt;=0</t>
   </si>
   <si>
-    <t>$B$2:$D$2</t>
-  </si>
-  <si>
-    <t>$E$3:$E$5 &gt;= $F$3:$F$5</t>
-  </si>
-  <si>
-    <t>$B$2:$D$2 &gt;= 0</t>
-  </si>
-  <si>
     <t>Microsoft Excel 16.0 Отчет об устойчивости</t>
   </si>
   <si>
@@ -304,12 +292,6 @@
     <t>-v</t>
   </si>
   <si>
-    <t>Отчет создан: 16.10.2021 19:56:17</t>
-  </si>
-  <si>
-    <t>Число итераций: 3 Число подзадач: 0</t>
-  </si>
-  <si>
     <t>$E$2</t>
   </si>
   <si>
@@ -323,18 +305,44 @@
   </si>
   <si>
     <t>yi</t>
+  </si>
+  <si>
+    <t>Лист: [Lab3.1.xlsx]Поиск решения</t>
+  </si>
+  <si>
+    <t>Отчет создан: 18.10.2021 13:54:53</t>
+  </si>
+  <si>
+    <t>Число итераций: 5 Число подзадач: 0</t>
+  </si>
+  <si>
+    <t>yi П1</t>
+  </si>
+  <si>
+    <t>yi П2</t>
+  </si>
+  <si>
+    <t>yi П3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -357,17 +365,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="18"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color indexed="18"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -384,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -826,32 +834,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1174,12 +1156,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1214,9 +1205,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
@@ -1228,54 +1219,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="49" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1559,25 +1539,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64"/>
-      <c r="B1" s="57" t="s">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="59"/>
+      <c r="B1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1588,13 +1568,13 @@
         <v>12</v>
       </c>
       <c r="D2" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -1611,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -1628,21 +1608,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="45">
         <v>0.2</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="46">
         <v>0.65</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="47">
         <v>0.16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1650,8 +1630,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="25" t="s">
         <v>6</v>
@@ -1668,17 +1648,17 @@
       <c r="F9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="50" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="24"/>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="40" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="28" t="s">
@@ -1687,11 +1667,11 @@
       <c r="N9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="52" t="s">
+      <c r="O9" s="50" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>3</v>
       </c>
@@ -1702,11 +1682,11 @@
         <v>12</v>
       </c>
       <c r="D10" s="23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3">
         <f>MIN(B10:D10)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F10" s="17">
         <f>MAX(B10:D10)</f>
@@ -1714,9 +1694,9 @@
       </c>
       <c r="G10" s="14">
         <f>$C$7*E10+F10*(1-$C$7)</f>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="I10" s="37" t="s">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I10" s="35" t="s">
         <v>3</v>
       </c>
       <c r="J10" s="3">
@@ -1729,7 +1709,7 @@
       </c>
       <c r="L10" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M10" s="11">
         <f>MIN(J10:L10)</f>
@@ -1737,14 +1717,14 @@
       </c>
       <c r="N10" s="17">
         <f>MAX(J10:L10)</f>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="O10" s="20">
         <f>$C$7*M10+N10*(1-$C$7)</f>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>4</v>
       </c>
@@ -1769,7 +1749,7 @@
         <f t="shared" ref="G11:G12" si="3">$C$7*E11+F11*(1-$C$7)</f>
         <v>9.8000000000000007</v>
       </c>
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="36" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="6">
@@ -1797,7 +1777,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="30" t="s">
         <v>5</v>
       </c>
@@ -1810,19 +1790,19 @@
       <c r="D12" s="33">
         <v>18</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="51">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="52">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="49">
         <f t="shared" si="3"/>
         <v>13.8</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J12" s="8">
@@ -1841,16 +1821,16 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N12" s="55">
+      <c r="N12" s="52">
         <f>MAX(J12:L12)</f>
         <v>3</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="49">
         <f t="shared" si="5"/>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>11</v>
       </c>
@@ -1866,46 +1846,46 @@
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="53" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="40" t="s">
+      <c r="K15" s="38" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="3">
@@ -1918,34 +1898,34 @@
       </c>
       <c r="D16" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="E16" s="14">
         <f>SUM(B16:D16)</f>
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="G16" s="37" t="s">
+        <v>11.200000000000001</v>
+      </c>
+      <c r="G16" s="35" t="s">
         <v>3</v>
       </c>
       <c r="H16" s="3">
-        <f>(B$13-B16)*H$19</f>
-        <v>2.64</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" ref="I16:J16" si="8">(C$13-C16)*I$19</f>
-        <v>4.0299999999999994</v>
-      </c>
-      <c r="J16" s="5">
+        <f>J10*H$19</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16:J16" si="8">K10*I$19</f>
+        <v>1.3</v>
+      </c>
+      <c r="J16" s="3">
         <f t="shared" si="8"/>
-        <v>2.88</v>
-      </c>
-      <c r="K16" s="58">
+        <v>1.28</v>
+      </c>
+      <c r="K16" s="55">
         <f>SUM(H16:J16)</f>
-        <v>9.5500000000000007</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+        <v>3.7800000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="6">
@@ -1964,28 +1944,28 @@
         <f t="shared" ref="E17:E18" si="9">SUM(B17:D17)</f>
         <v>11.94</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="6">
-        <f t="shared" ref="H17:H18" si="10">(B$13-B17)*H$19</f>
-        <v>2.72</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" ref="I17:I18" si="11">(C$13-C17)*I$19</f>
-        <v>3.1850000000000005</v>
-      </c>
-      <c r="J17" s="7">
-        <f t="shared" ref="J17:J18" si="12">(D$13-D17)*J$19</f>
-        <v>2.6496</v>
-      </c>
-      <c r="K17" s="62">
+      <c r="H17" s="3">
+        <f t="shared" ref="H17:H18" si="10">J11*H$19</f>
+        <v>1.6</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" ref="I17:I18" si="11">K11*I$19</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" ref="J17:J18" si="12">L11*J$19</f>
+        <v>1.44</v>
+      </c>
+      <c r="K17" s="76">
         <f>SUM(H17:J17)</f>
-        <v>8.5546000000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="42" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="8">
@@ -2000,32 +1980,32 @@
         <f t="shared" si="7"/>
         <v>2.88</v>
       </c>
-      <c r="E18" s="61">
+      <c r="E18" s="57">
         <f t="shared" si="9"/>
         <v>13.030000000000001</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="3">
         <f t="shared" si="10"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="I18" s="9">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
         <f t="shared" si="11"/>
-        <v>4.4524999999999997</v>
-      </c>
-      <c r="J18" s="10">
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="J18" s="3">
         <f t="shared" si="12"/>
-        <v>2.4192</v>
-      </c>
-      <c r="K18" s="59">
+        <v>0</v>
+      </c>
+      <c r="K18" s="74">
         <f>SUM(H18:J18)</f>
-        <v>9.2716999999999992</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="45" t="s">
+        <v>1.9500000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="28">
@@ -2037,177 +2017,177 @@
       <c r="D19" s="29">
         <v>0.16</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="50" t="s">
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="47">
+      <c r="H19" s="45">
         <v>0.2</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="46">
         <v>0.65</v>
       </c>
-      <c r="J19" s="49">
+      <c r="J19" s="47">
         <v>0.16</v>
       </c>
-      <c r="K19" s="36"/>
-      <c r="N19" s="36"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="34"/>
+      <c r="N19" s="34"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="63" t="s">
+      <c r="E21" s="58" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="24"/>
-      <c r="H21" s="57" t="s">
+      <c r="H21" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="60" t="s">
+      <c r="J21" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="40" t="s">
+      <c r="K21" s="38" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" ref="B22:D24" si="13">B16*B$19</f>
-        <v>0.36000000000000004</v>
-      </c>
-      <c r="C22" s="4">
+        <f>B10*B$19</f>
+        <v>1.8</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" ref="C22:D22" si="13">C10*C$19</f>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="D22" s="3">
         <f t="shared" si="13"/>
-        <v>5.07</v>
-      </c>
-      <c r="D22" s="17">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="E22" s="14">
         <f>SUM(B22:D22)</f>
-        <v>5.4300000000000006</v>
-      </c>
-      <c r="G22" s="37" t="s">
+        <v>11.200000000000001</v>
+      </c>
+      <c r="G22" s="35" t="s">
         <v>3</v>
       </c>
       <c r="H22" s="3">
-        <f>(B$13-B22)*H$19</f>
-        <v>2.9280000000000004</v>
-      </c>
-      <c r="I22" s="4">
-        <f t="shared" ref="I22:I24" si="14">(C$13-C22)*I$19</f>
-        <v>5.8045</v>
-      </c>
-      <c r="J22" s="5">
-        <f t="shared" ref="J22:J24" si="15">(D$13-D22)*J$19</f>
+        <f>J10*B$25</f>
+        <v>2</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" ref="I22:J22" si="14">K10*C$25</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="14"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="K22" s="55">
+        <f>SUM(H22:J22)</f>
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" ref="B23:D23" si="15">B11*B$19</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="15"/>
+        <v>9.1</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="15"/>
+        <v>1.44</v>
+      </c>
+      <c r="E23" s="75">
+        <f t="shared" ref="E23:E24" si="16">SUM(B23:D23)</f>
+        <v>11.94</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" ref="H23:H24" si="17">J11*B$25</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" ref="I23:I24" si="18">K11*C$25</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" ref="J23:J24" si="19">L11*D$25</f>
+        <v>3</v>
+      </c>
+      <c r="K23" s="76">
+        <f>SUM(H23:J23)</f>
+        <v>5.6666666666666661</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" ref="B24:D24" si="20">B12*B$19</f>
+        <v>3</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="20"/>
+        <v>7.15</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="20"/>
         <v>2.88</v>
       </c>
-      <c r="K22" s="58">
-        <f>SUM(H22:J22)</f>
-        <v>11.612500000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="6">
-        <f t="shared" si="13"/>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C23" s="2">
-        <f t="shared" si="13"/>
-        <v>5.915</v>
-      </c>
-      <c r="D23" s="18">
-        <f t="shared" si="13"/>
-        <v>0.23039999999999999</v>
-      </c>
-      <c r="E23" s="53">
-        <f t="shared" ref="E23:E24" si="16">SUM(B23:D23)</f>
-        <v>6.4254000000000007</v>
-      </c>
-      <c r="G23" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="6">
-        <f t="shared" ref="H23:H24" si="17">(B$13-B23)*H$19</f>
-        <v>2.9440000000000004</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="14"/>
-        <v>5.2552500000000011</v>
-      </c>
-      <c r="J23" s="7">
-        <f t="shared" si="15"/>
-        <v>2.8431360000000003</v>
-      </c>
-      <c r="K23" s="62">
-        <f>SUM(H23:J23)</f>
-        <v>11.042386</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="44" t="s">
+      <c r="E24" s="49">
+        <f t="shared" si="16"/>
+        <v>13.030000000000001</v>
+      </c>
+      <c r="G24" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="34">
-        <f t="shared" si="13"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="C24" s="32">
-        <f t="shared" si="13"/>
-        <v>4.6475</v>
-      </c>
-      <c r="D24" s="33">
-        <f t="shared" si="13"/>
-        <v>0.46079999999999999</v>
-      </c>
-      <c r="E24" s="16">
-        <f t="shared" si="16"/>
-        <v>5.7083000000000004</v>
-      </c>
-      <c r="G24" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="34">
+      <c r="H24" s="3">
         <f t="shared" si="17"/>
-        <v>2.8800000000000003</v>
-      </c>
-      <c r="I24" s="32">
-        <f t="shared" si="14"/>
-        <v>6.0791249999999994</v>
-      </c>
-      <c r="J24" s="35">
-        <f t="shared" si="15"/>
-        <v>2.8062720000000003</v>
-      </c>
-      <c r="K24" s="59">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="74">
         <f>SUM(H24:J24)</f>
-        <v>11.765397</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="28">
@@ -2215,16 +2195,16 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C25" s="26">
-        <f t="shared" ref="C25:D25" si="18">1/COUNT($B22:$D22)</f>
+        <f t="shared" ref="C25:D25" si="21">1/COUNT($B22:$D22)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="D25" s="29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="50" t="s">
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H25" s="28">
@@ -2232,14 +2212,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="I25" s="26">
-        <f t="shared" ref="I25:J25" si="19">1/COUNT($H22:$J22)</f>
+        <f t="shared" ref="I25:J25" si="22">1/COUNT($H22:$J22)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="J25" s="29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K25" s="36"/>
+      <c r="K25" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2249,380 +2229,329 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="60" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="60"/>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="60"/>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="60"/>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="61" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65"/>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" collapsed="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D16" s="63">
+        <v>8.6419753086419776E-2</v>
+      </c>
+      <c r="E16" s="63">
+        <v>8.4905660377358499E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="69" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="67" t="s">
+      <c r="C20" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="D20" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="E20" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="67" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="70">
-        <v>8.6419753086419748E-2</v>
-      </c>
-      <c r="E16" s="70">
-        <v>8.6419753086419748E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="F20" s="69" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="67" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="64">
+        <v>1.2345679012345699E-2</v>
+      </c>
+      <c r="E21" s="64">
+        <v>0</v>
+      </c>
+      <c r="F21" s="62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="64">
+        <v>7.4074074074074084E-2</v>
+      </c>
+      <c r="E22" s="64">
+        <v>7.5471698113207558E-2</v>
+      </c>
+      <c r="F22" s="62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="63">
+        <v>0</v>
+      </c>
+      <c r="E23" s="63">
+        <v>9.4339622641509361E-3</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="67" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-    </row>
-    <row r="22" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="71">
-        <v>1.2345679012345671E-2</v>
-      </c>
-      <c r="E22" s="71">
-        <v>1.2345679012345671E-2</v>
-      </c>
-      <c r="F22" s="69" t="s">
+      <c r="D27" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="69" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="64">
+        <v>1</v>
+      </c>
+      <c r="E28" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="64">
+        <v>1.1415094339622642</v>
+      </c>
+      <c r="E29" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="64">
+        <v>0.14150943396226423</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="64">
+        <v>1</v>
+      </c>
+      <c r="E30" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="64">
+        <v>0</v>
+      </c>
+      <c r="E31" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="62" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="69" t="s">
+      <c r="C32" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="64">
+        <v>7.5471698113207558E-2</v>
+      </c>
+      <c r="E32" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="64">
+        <v>7.5471698113207558E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="71">
-        <v>7.4074074074074084E-2</v>
-      </c>
-      <c r="E23" s="71">
-        <v>7.4074074074074084E-2</v>
-      </c>
-      <c r="F23" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="70">
-        <v>0</v>
-      </c>
-      <c r="E24" s="70">
-        <v>0</v>
-      </c>
-      <c r="F24" s="66" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="68"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="67" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-    </row>
-    <row r="31" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="71">
-        <v>1</v>
-      </c>
-      <c r="E31" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="71">
-        <v>1.1234567901234569</v>
-      </c>
-      <c r="E32" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="G32" s="71">
-        <v>0.12345679012345689</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="69" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="71">
-        <v>1</v>
-      </c>
-      <c r="E33" s="69" t="s">
+      <c r="C33" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="63">
+        <v>9.4339622641509361E-3</v>
+      </c>
+      <c r="E33" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="F33" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33" s="71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="71"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="75" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="69"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="71"/>
-    </row>
-    <row r="36" spans="2:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="71">
-        <v>1.2345679012345671E-2</v>
-      </c>
-      <c r="E36" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="G36" s="71">
-        <v>1.2345679012345671E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="71">
-        <v>7.4074074074074084E-2</v>
-      </c>
-      <c r="E37" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" s="71">
-        <v>7.4074074074074084E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="70">
-        <v>0</v>
-      </c>
-      <c r="E38" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="72"/>
+      <c r="G33" s="63">
+        <v>9.4339622641509361E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2631,310 +2560,270 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E21" sqref="E19:E21"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="71" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="76" t="s">
+      <c r="F8" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="62">
+        <v>0</v>
+      </c>
+      <c r="E9" s="62">
+        <v>0.12264150943396229</v>
+      </c>
+      <c r="F9" s="62">
+        <v>1</v>
+      </c>
+      <c r="G9" s="62">
+        <v>1E+30</v>
+      </c>
+      <c r="H9" s="62">
+        <v>0.12264150943396229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="62">
+        <v>7.5471698113207558E-2</v>
+      </c>
+      <c r="E10" s="62">
+        <v>0</v>
+      </c>
+      <c r="F10" s="62">
+        <v>1</v>
+      </c>
+      <c r="G10" s="62">
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="H10" s="62">
+        <v>0.38888888888888878</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="61">
+        <v>9.4339622641509361E-3</v>
+      </c>
+      <c r="E11" s="61">
+        <v>0</v>
+      </c>
+      <c r="F11" s="61">
+        <v>1</v>
+      </c>
+      <c r="G11" s="61">
+        <v>0.1604938271604939</v>
+      </c>
+      <c r="H11" s="61">
+        <v>0.16666666666666674</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="H14" s="70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="76" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="77" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="77" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="77" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-    </row>
-    <row r="10" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="69">
-        <v>1.2345679012345671E-2</v>
-      </c>
-      <c r="E10" s="69">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="62">
+        <v>1</v>
+      </c>
+      <c r="E16" s="62">
+        <v>6.6037735849056589E-2</v>
+      </c>
+      <c r="F16" s="62">
+        <v>1</v>
+      </c>
+      <c r="G16" s="62">
+        <v>9.0909090909090842E-2</v>
+      </c>
+      <c r="H16" s="62">
+        <v>9.803921568627455E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="62">
+        <v>1.1415094339622642</v>
+      </c>
+      <c r="E17" s="62">
         <v>0</v>
       </c>
-      <c r="F10" s="69">
+      <c r="F17" s="62">
         <v>1</v>
       </c>
-      <c r="G10" s="69">
-        <v>0.125</v>
-      </c>
-      <c r="H10" s="69">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="69">
-        <v>7.4074074074074084E-2</v>
-      </c>
-      <c r="E11" s="69">
-        <v>0</v>
-      </c>
-      <c r="F11" s="69">
+      <c r="G17" s="62">
+        <v>0.14150943396226423</v>
+      </c>
+      <c r="H17" s="62">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="61">
         <v>1</v>
       </c>
-      <c r="G11" s="69">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="H11" s="69">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="66">
-        <v>0</v>
-      </c>
-      <c r="E12" s="66">
-        <v>0.33333333333333326</v>
-      </c>
-      <c r="F12" s="66">
+      <c r="E18" s="61">
+        <v>1.8867924528301893E-2</v>
+      </c>
+      <c r="F18" s="61">
         <v>1</v>
       </c>
-      <c r="G12" s="66">
-        <v>1E+30</v>
-      </c>
-      <c r="H12" s="66">
-        <v>0.33333333333333326</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="76" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="76" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="77" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="77" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-    </row>
-    <row r="19" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="69">
-        <v>1</v>
-      </c>
-      <c r="E19" s="69">
-        <v>4.9382716049382713E-2</v>
-      </c>
-      <c r="F19" s="69">
-        <v>1</v>
-      </c>
-      <c r="G19" s="69">
-        <v>9.0909090909090856E-2</v>
-      </c>
-      <c r="H19" s="69">
-        <v>7.5187969924812081E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="69">
-        <v>1.1234567901234569</v>
-      </c>
-      <c r="E20" s="69">
-        <v>0</v>
-      </c>
-      <c r="F20" s="69">
-        <v>1</v>
-      </c>
-      <c r="G20" s="69">
-        <v>0.12345679012345687</v>
-      </c>
-      <c r="H20" s="69">
-        <v>1E+30</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="66">
-        <v>1</v>
-      </c>
-      <c r="E21" s="66">
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="F21" s="66">
-        <v>1</v>
-      </c>
-      <c r="G21" s="66">
-        <v>0.23809523809523825</v>
-      </c>
-      <c r="H21" s="66">
-        <v>8.3333333333333287E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
+      <c r="G18" s="61">
+        <v>0.46875</v>
+      </c>
+      <c r="H18" s="61">
+        <v>8.3333333333333273E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2949,173 +2838,175 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="70"/>
+      <c r="C6" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="70"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="63">
+        <v>8.4905660377358499E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="70"/>
+      <c r="C11" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="70"/>
+      <c r="F11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="71" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="76"/>
-      <c r="C6" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="76"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="77" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="70">
-        <v>8.6419753086419748E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="76"/>
-      <c r="C11" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="76"/>
-      <c r="F11" s="76" t="s">
+      <c r="I12" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="64">
+        <v>0</v>
+      </c>
+      <c r="F13" s="64">
+        <v>0</v>
+      </c>
+      <c r="G13" s="64">
+        <v>8.4905660377358499E-2</v>
+      </c>
+      <c r="I13" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="76" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="77" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="77" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="77" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" s="77" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="71">
-        <v>1.2345679012345671E-2</v>
-      </c>
-      <c r="F13" s="71">
-        <v>1.2345679012345659E-2</v>
-      </c>
-      <c r="G13" s="71">
-        <v>8.6419753086419748E-2</v>
-      </c>
-      <c r="I13" s="69" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="69" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="69" t="s">
+      <c r="J13" s="62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="64">
+        <v>7.5471698113207558E-2</v>
+      </c>
+      <c r="F14" s="64">
+        <v>7.5471698113207544E-2</v>
+      </c>
+      <c r="G14" s="64">
+        <v>8.4905660377358486E-2</v>
+      </c>
+      <c r="I14" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="71">
-        <v>7.4074074074074084E-2</v>
-      </c>
-      <c r="F14" s="71">
-        <v>7.407407407407407E-2</v>
-      </c>
-      <c r="G14" s="71">
-        <v>8.6419753086419748E-2</v>
-      </c>
-      <c r="I14" s="69" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="69" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="70">
-        <v>0</v>
-      </c>
-      <c r="F15" s="70">
-        <v>0</v>
-      </c>
-      <c r="G15" s="70">
-        <v>8.6419753086419748E-2</v>
-      </c>
-      <c r="I15" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="66" t="s">
-        <v>78</v>
+      <c r="C15" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="63">
+        <v>9.4339622641509361E-3</v>
+      </c>
+      <c r="F15" s="63">
+        <v>9.4339622641509309E-3</v>
+      </c>
+      <c r="G15" s="63">
+        <v>8.4905660377358486E-2</v>
+      </c>
+      <c r="I15" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="61" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3128,55 +3019,54 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="7" max="7" width="2.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64"/>
-      <c r="B1" s="57" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="59"/>
+      <c r="B1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B2">
-        <v>1.2345679012345699E-2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>7.4074074074074084E-2</v>
+        <v>7.5471698113207558E-2</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="65">
+        <v>9.4339622641509361E-3</v>
+      </c>
+      <c r="E2" s="60">
         <f>SUM(B$2:D$2)</f>
-        <v>8.6419753086419776E-2</v>
-      </c>
-      <c r="F2" s="65">
+        <v>8.4905660377358499E-2</v>
+      </c>
+      <c r="F2" s="60">
         <f>1/E2</f>
-        <v>11.571428571428568</v>
+        <v>11.777777777777777</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -3187,17 +3077,17 @@
         <v>12</v>
       </c>
       <c r="D3" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <f>SUMPRODUCT(B$2:D$2,B3:D3)</f>
-        <v>1.0000000000000004</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
@@ -3212,13 +3102,13 @@
       </c>
       <c r="E4">
         <f>SUMPRODUCT(B$2:D$2,B4:D4)</f>
-        <v>1.1234567901234571</v>
+        <v>1.1415094339622642</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
@@ -3233,72 +3123,77 @@
       </c>
       <c r="E5">
         <f>SUMPRODUCT(B$2:D$2,B5:D5)</f>
-        <v>1.0000000000000004</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="65">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="60">
         <f>$F$2*B2</f>
-        <v>0.14285714285714304</v>
-      </c>
-      <c r="C6" s="65">
+        <v>0</v>
+      </c>
+      <c r="C6" s="60">
         <f t="shared" ref="C6:D6" si="0">$F$2*C2</f>
-        <v>0.85714285714285698</v>
-      </c>
-      <c r="D6" s="65">
+        <v>0.88888888888888895</v>
+      </c>
+      <c r="D6" s="60">
         <f t="shared" si="0"/>
+        <v>0.11111111111111102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="67">
+        <v>6.6037735849056603E-2</v>
+      </c>
+      <c r="C8" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="80">
-        <v>4.9382716049382713E-2</v>
-      </c>
-      <c r="C8" s="80">
-        <v>0</v>
-      </c>
-      <c r="D8" s="80">
-        <v>3.7037037037037035E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="81">
+      <c r="D8" s="67">
+        <v>1.88679245283019E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="68">
         <f>$F$2*B8</f>
-        <v>0.57142857142857117</v>
-      </c>
-      <c r="C9" s="81">
+        <v>0.77777777777777768</v>
+      </c>
+      <c r="C9" s="68">
         <f t="shared" ref="C9:D9" si="1">$F$2*C8</f>
         <v>0</v>
       </c>
-      <c r="D9" s="81">
+      <c r="D9" s="72">
         <f t="shared" si="1"/>
-        <v>0.42857142857142838</v>
+        <v>0.22222222222222235</v>
       </c>
       <c r="E9">
         <f>SUM(B9:D9)</f>
-        <v>0.99999999999999956</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="78"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="78"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="78"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="73"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="65"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="65"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>